<commit_message>
add function on count files
</commit_message>
<xml_diff>
--- a/backend/test.xlsx
+++ b/backend/test.xlsx
@@ -10,14 +10,14 @@
     <sheet name="Лист1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$3:$G$393</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Лист1!$A$3:$G$392</definedName>
   </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="22">
   <si>
     <t>"Все Свои (229-01-45)"</t>
   </si>
@@ -82,19 +82,10 @@
     <t>Запись разговора</t>
   </si>
   <si>
-    <t>26.02.2025 07:31:39</t>
-  </si>
-  <si>
     <t>Входящий</t>
   </si>
   <si>
-    <t>79296304300</t>
-  </si>
-  <si>
     <t>ДМТ-SIP-Москва-контекст</t>
-  </si>
-  <si>
-    <t>[kos] Гынку Анастасия</t>
   </si>
   <si>
     <t>Прочие звонки</t>
@@ -1035,11 +1026,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G393"/>
+  <dimension ref="A1:G392"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="3" topLeftCell="A4" activePane="bottomLeft" state="frozenSplit"/>
-      <selection pane="bottomLeft" activeCell="A8" sqref="A8:G393"/>
+      <selection pane="bottomLeft" activeCell="A4" sqref="A4:XFD4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -1088,25 +1079,25 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="B4" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="4" t="s">
+      <c r="C4" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="E4" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F4" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="4" t="s">
+      <c r="G4" s="5" t="s">
         <v>12</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -1114,69 +1105,55 @@
         <v>16</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C5" s="4" t="s">
         <v>17</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G5" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E5" s="4" t="s">
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="F5" s="4" t="s">
-        <v>14</v>
+      <c r="B6" s="4" t="s">
+        <v>9</v>
       </c>
-      <c r="G5" s="5" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A6" s="4" t="s">
+      <c r="C6" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C6" s="4" t="s">
+      <c r="D6" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="D6" s="4" t="s">
+      <c r="E6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="F6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="E6" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G6" s="5" t="s">
-        <v>15</v>
-      </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A7" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="G7" s="5" t="s">
-        <v>15</v>
-      </c>
+      <c r="A7" s="4"/>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="4"/>
@@ -1491,7 +1468,7 @@
       <c r="D42" s="4"/>
       <c r="E42" s="4"/>
       <c r="F42" s="4"/>
-      <c r="G42" s="5"/>
+      <c r="G42" s="4"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="4"/>
@@ -1500,7 +1477,7 @@
       <c r="D43" s="4"/>
       <c r="E43" s="4"/>
       <c r="F43" s="4"/>
-      <c r="G43" s="4"/>
+      <c r="G43" s="5"/>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="4"/>
@@ -4643,22 +4620,12 @@
       <c r="F392" s="4"/>
       <c r="G392" s="5"/>
     </row>
-    <row r="393" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A393" s="4"/>
-      <c r="B393" s="4"/>
-      <c r="C393" s="4"/>
-      <c r="D393" s="4"/>
-      <c r="E393" s="4"/>
-      <c r="F393" s="4"/>
-      <c r="G393" s="5"/>
-    </row>
   </sheetData>
-  <autoFilter ref="A3:G393"/>
+  <autoFilter ref="A3:G392"/>
   <hyperlinks>
-    <hyperlink ref="G4" r:id="rId1" display="https://sc.wilstream.ru/sc/get_okt_record.php?idchain=771fe790-1ad2-4f09-8514-95a5f14cc371&amp;acc=83e937b5&amp;datecall=20250226-073139"/>
-    <hyperlink ref="G5" r:id="rId2" display="https://sc.wilstream.ru/sc/get_okt_record.php?idchain=154c548c-3011-486b-be3b-b3629568cf83&amp;acc=09d5eaab&amp;datecall=20250226-074933"/>
-    <hyperlink ref="G6" r:id="rId3" display="https://sc.wilstream.ru/sc/get_okt_record.php?idchain=54cfa2cd-1677-4a7b-a5d7-2e8c09e43a46&amp;acc=1985f371&amp;datecall=20250226-075912"/>
-    <hyperlink ref="G7" r:id="rId4" display="https://sc.wilstream.ru/sc/get_okt_record.php?idchain=02a3bcc2-d940-458c-8765-12fa6ed9094a&amp;acc=cd8a2d44&amp;datecall=20250226-080002"/>
+    <hyperlink ref="G4" r:id="rId1" display="https://sc.wilstream.ru/sc/get_okt_record.php?idchain=154c548c-3011-486b-be3b-b3629568cf83&amp;acc=09d5eaab&amp;datecall=20250226-074933"/>
+    <hyperlink ref="G5" r:id="rId2" display="https://sc.wilstream.ru/sc/get_okt_record.php?idchain=54cfa2cd-1677-4a7b-a5d7-2e8c09e43a46&amp;acc=1985f371&amp;datecall=20250226-075912"/>
+    <hyperlink ref="G6" r:id="rId3" display="https://sc.wilstream.ru/sc/get_okt_record.php?idchain=02a3bcc2-d940-458c-8765-12fa6ed9094a&amp;acc=cd8a2d44&amp;datecall=20250226-080002"/>
   </hyperlinks>
   <pageMargins left="0.79" right="0.79" top="0.98" bottom="0.98" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>